<commit_message>
new dataset spike and pickle
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phbro\Desktop\DOCUMENTS\ActuRank\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA20ACE0-2A75-4E2F-9486-E866A56A3838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B49F7-017B-481D-90C0-3688D5E47258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="0" windowWidth="21924" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1008" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="99">
   <si>
     <t>players</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>20/08/2024</t>
+  </si>
+  <si>
+    <t>27/08/2024</t>
   </si>
 </sst>
 </file>
@@ -721,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O959"/>
+  <dimension ref="A1:O967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A933" workbookViewId="0">
-      <selection activeCell="F951" sqref="F951"/>
+    <sheetView tabSelected="1" topLeftCell="A947" workbookViewId="0">
+      <selection activeCell="J966" sqref="J966"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25605,7 +25608,7 @@
       </c>
       <c r="D720" s="7"/>
       <c r="E720" s="1">
-        <f t="shared" ref="E720:E951" si="23">IF(F720&gt;G720,1,0)</f>
+        <f t="shared" ref="E720:E937" si="23">IF(F720&gt;G720,1,0)</f>
         <v>1</v>
       </c>
       <c r="F720" s="5">
@@ -29669,7 +29672,7 @@
         <v>89</v>
       </c>
       <c r="K856" s="10" t="str">
-        <f t="shared" ref="K856:K937" si="25">IF(OR(OR(AND(OR(A856=B856,A856=C856,A856=D856,B856=C856,B856=D856,C856=D856),OR(A856&lt;&gt;"",D856&lt;&gt;"")),H856&gt;MAX(F856:G856),B856=C856),OR(AND(ISBLANK(A856)=FALSE,ISNA(VLOOKUP(A856,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B856,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C856,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D856)=FALSE,ISNA(VLOOKUP(D856,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A856:D856)=1,COUNTBLANK(A856:D856)=3))),"ERREUR","")</f>
+        <f t="shared" ref="K856:K938" si="25">IF(OR(OR(AND(OR(A856=B856,A856=C856,A856=D856,B856=C856,B856=D856,C856=D856),OR(A856&lt;&gt;"",D856&lt;&gt;"")),H856&gt;MAX(F856:G856),B856=C856),OR(AND(ISBLANK(A856)=FALSE,ISNA(VLOOKUP(A856,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B856,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C856,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D856)=FALSE,ISNA(VLOOKUP(D856,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A856:D856)=1,COUNTBLANK(A856:D856)=3))),"ERREUR","")</f>
         <v/>
       </c>
     </row>
@@ -31964,6 +31967,10 @@
       <c r="I938" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K938" s="10" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
     </row>
     <row r="939" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B939" s="6" t="s">
@@ -31988,6 +31995,10 @@
       <c r="I939" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K939" s="10" t="str">
+        <f t="shared" ref="K939:K967" si="27">IF(OR(OR(AND(OR(A939=B939,A939=C939,A939=D939,B939=C939,B939=D939,C939=D939),OR(A939&lt;&gt;"",D939&lt;&gt;"")),H939&gt;MAX(F939:G939),B939=C939),OR(AND(ISBLANK(A939)=FALSE,ISNA(VLOOKUP(A939,$M$3:$O$27,1,FALSE))),ISNA(VLOOKUP(B939,$M$3:$O$27,1,FALSE)),ISNA(VLOOKUP(C939,$M$3:$O$27,1,FALSE)),AND(ISBLANK(D939)=FALSE,ISNA(VLOOKUP(D939,$M$3:$O$27,1,FALSE))),OR(COUNTBLANK(A939:D939)=1,COUNTBLANK(A939:D939)=3))),"ERREUR","")</f>
+        <v/>
+      </c>
     </row>
     <row r="940" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B940" s="6" t="s">
@@ -32012,6 +32023,10 @@
       <c r="I940" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K940" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
     </row>
     <row r="941" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B941" s="6" t="s">
@@ -32021,7 +32036,7 @@
         <v>14</v>
       </c>
       <c r="E941" s="1">
-        <f>IF(F941&gt;G941,1,0)</f>
+        <f t="shared" ref="E941:E967" si="28">IF(F941&gt;G941,1,0)</f>
         <v>1</v>
       </c>
       <c r="F941" s="5">
@@ -32036,6 +32051,10 @@
       <c r="I941" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K941" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
     </row>
     <row r="942" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B942" s="6" t="s">
@@ -32045,7 +32064,7 @@
         <v>22</v>
       </c>
       <c r="E942" s="1">
-        <f>IF(F942&gt;G942,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F942" s="5">
@@ -32060,6 +32079,10 @@
       <c r="I942" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K942" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
     </row>
     <row r="943" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B943" s="6" t="s">
@@ -32069,7 +32092,7 @@
         <v>12</v>
       </c>
       <c r="E943" s="1">
-        <f>IF(F943&gt;G943,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F943" s="5">
@@ -32084,6 +32107,10 @@
       <c r="I943" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="K943" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
     </row>
     <row r="944" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B944" s="6" t="s">
@@ -32093,7 +32120,7 @@
         <v>22</v>
       </c>
       <c r="E944" s="1">
-        <f>IF(F944&gt;G944,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F944" s="5">
@@ -32108,8 +32135,12 @@
       <c r="I944" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="945" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K944" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="945" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B945" s="6" t="s">
         <v>14</v>
       </c>
@@ -32117,7 +32148,7 @@
         <v>12</v>
       </c>
       <c r="E945" s="1">
-        <f>IF(F945&gt;G945,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F945" s="5">
@@ -32132,8 +32163,12 @@
       <c r="I945" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="946" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K945" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="946" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B946" s="6" t="s">
         <v>14</v>
       </c>
@@ -32141,7 +32176,7 @@
         <v>22</v>
       </c>
       <c r="E946" s="1">
-        <f>IF(F946&gt;G946,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F946" s="5">
@@ -32156,8 +32191,12 @@
       <c r="I946" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="947" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K946" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="947" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B947" s="6" t="s">
         <v>12</v>
       </c>
@@ -32165,7 +32204,7 @@
         <v>22</v>
       </c>
       <c r="E947" s="1">
-        <f>IF(F947&gt;G947,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F947" s="5">
@@ -32180,8 +32219,12 @@
       <c r="I947" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="948" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K947" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="948" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B948" s="6" t="s">
         <v>14</v>
       </c>
@@ -32189,7 +32232,7 @@
         <v>12</v>
       </c>
       <c r="E948" s="1">
-        <f>IF(F948&gt;G948,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F948" s="5">
@@ -32204,8 +32247,12 @@
       <c r="I948" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="949" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K948" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="949" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B949" s="6" t="s">
         <v>14</v>
       </c>
@@ -32213,7 +32260,7 @@
         <v>22</v>
       </c>
       <c r="E949" s="1">
-        <f>IF(F949&gt;G949,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F949" s="5">
@@ -32228,8 +32275,12 @@
       <c r="I949" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="950" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K949" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="950" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B950" s="6" t="s">
         <v>14</v>
       </c>
@@ -32237,7 +32288,7 @@
         <v>11</v>
       </c>
       <c r="E950" s="1">
-        <f>IF(F950&gt;G950,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F950" s="5">
@@ -32252,8 +32303,12 @@
       <c r="I950" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="951" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K950" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="951" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B951" s="6" t="s">
         <v>14</v>
       </c>
@@ -32261,7 +32316,7 @@
         <v>22</v>
       </c>
       <c r="E951" s="1">
-        <f>IF(F951&gt;G951,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F951" s="5">
@@ -32276,8 +32331,12 @@
       <c r="I951" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="952" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K951" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="952" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B952" s="6" t="s">
         <v>14</v>
       </c>
@@ -32285,7 +32344,7 @@
         <v>11</v>
       </c>
       <c r="E952" s="1">
-        <f>IF(F952&gt;G952,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F952" s="5">
@@ -32300,8 +32359,12 @@
       <c r="I952" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="953" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K952" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="953" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B953" s="6" t="s">
         <v>22</v>
       </c>
@@ -32309,7 +32372,7 @@
         <v>11</v>
       </c>
       <c r="E953" s="1">
-        <f>IF(F953&gt;G953,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F953" s="5">
@@ -32324,8 +32387,12 @@
       <c r="I953" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="954" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K953" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="954" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B954" s="6" t="s">
         <v>14</v>
       </c>
@@ -32333,7 +32400,7 @@
         <v>22</v>
       </c>
       <c r="E954" s="1">
-        <f>IF(F954&gt;G954,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F954" s="5">
@@ -32348,8 +32415,12 @@
       <c r="I954" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="955" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K954" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="955" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B955" s="6" t="s">
         <v>14</v>
       </c>
@@ -32357,7 +32428,7 @@
         <v>12</v>
       </c>
       <c r="E955" s="1">
-        <f>IF(F955&gt;G955,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F955" s="5">
@@ -32372,8 +32443,12 @@
       <c r="I955" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="956" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K955" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="956" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B956" s="6" t="s">
         <v>14</v>
       </c>
@@ -32381,7 +32456,7 @@
         <v>12</v>
       </c>
       <c r="E956" s="1">
-        <f>IF(F956&gt;G956,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F956" s="5">
@@ -32396,8 +32471,12 @@
       <c r="I956" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="957" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K956" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="957" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B957" s="6" t="s">
         <v>14</v>
       </c>
@@ -32405,7 +32484,7 @@
         <v>12</v>
       </c>
       <c r="E957" s="1">
-        <f>IF(F957&gt;G957,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F957" s="5">
@@ -32420,8 +32499,12 @@
       <c r="I957" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="958" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K957" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="958" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B958" s="6" t="s">
         <v>14</v>
       </c>
@@ -32429,7 +32512,7 @@
         <v>12</v>
       </c>
       <c r="E958" s="1">
-        <f>IF(F958&gt;G958,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F958" s="5">
@@ -32444,8 +32527,12 @@
       <c r="I958" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="959" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="K958" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="959" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B959" s="6" t="s">
         <v>14</v>
       </c>
@@ -32453,7 +32540,7 @@
         <v>12</v>
       </c>
       <c r="E959" s="1">
-        <f>IF(F959&gt;G959,1,0)</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F959" s="5">
@@ -32467,6 +32554,234 @@
       </c>
       <c r="I959" s="1" t="s">
         <v>97</v>
+      </c>
+      <c r="K959" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="960" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B960" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C960" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E960" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F960" s="5">
+        <v>5</v>
+      </c>
+      <c r="G960" s="5">
+        <v>2</v>
+      </c>
+      <c r="H960" s="1">
+        <v>5</v>
+      </c>
+      <c r="I960" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K960" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="961" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B961" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C961" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E961" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F961" s="5">
+        <v>5</v>
+      </c>
+      <c r="G961" s="5">
+        <v>0</v>
+      </c>
+      <c r="H961" s="1">
+        <v>5</v>
+      </c>
+      <c r="I961" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K961" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="962" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B962" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C962" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E962" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F962" s="5">
+        <v>5</v>
+      </c>
+      <c r="G962" s="5">
+        <v>1</v>
+      </c>
+      <c r="H962" s="1">
+        <v>5</v>
+      </c>
+      <c r="I962" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K962" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="963" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B963" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C963" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E963" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F963" s="5">
+        <v>7</v>
+      </c>
+      <c r="G963" s="5">
+        <v>5</v>
+      </c>
+      <c r="H963" s="1">
+        <v>5</v>
+      </c>
+      <c r="I963" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K963" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="964" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B964" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C964" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E964" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F964" s="5">
+        <v>7</v>
+      </c>
+      <c r="G964" s="5">
+        <v>5</v>
+      </c>
+      <c r="H964" s="1">
+        <v>5</v>
+      </c>
+      <c r="I964" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K964" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="965" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B965" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C965" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E965" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F965" s="5">
+        <v>5</v>
+      </c>
+      <c r="G965" s="5">
+        <v>2</v>
+      </c>
+      <c r="H965" s="1">
+        <v>5</v>
+      </c>
+      <c r="I965" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K965" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="966" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B966" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C966" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E966" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F966" s="5">
+        <v>5</v>
+      </c>
+      <c r="G966" s="5">
+        <v>3</v>
+      </c>
+      <c r="H966" s="1">
+        <v>5</v>
+      </c>
+      <c r="I966" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K966" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+    </row>
+    <row r="967" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B967" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C967" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E967" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="F967" s="5">
+        <v>5</v>
+      </c>
+      <c r="G967" s="5">
+        <v>2</v>
+      </c>
+      <c r="H967" s="1">
+        <v>5</v>
+      </c>
+      <c r="I967" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K967" s="10" t="str">
+        <f t="shared" si="27"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>